<commit_message>
Python for Data Analysis - Pandas Updated
</commit_message>
<xml_diff>
--- a/3_Pandas-Data_Analysis/My_Output_Excel.xlsx
+++ b/3_Pandas-Data_Analysis/My_Output_Excel.xlsx
@@ -383,91 +383,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>14</v>
-      </c>
-      <c r="E5">
         <v>15</v>
       </c>
     </row>

</xml_diff>